<commit_message>
update -> add function and comment
</commit_message>
<xml_diff>
--- a/excels/comment_list.xlsx
+++ b/excels/comment_list.xlsx
@@ -69,18 +69,18 @@
     <t>9</t>
   </si>
   <si>
-    <t>❤️❤️❤️</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>یعنی با وجود پیج من 😍😍😍😍😍😍
 .
 هنووووووزم صورتت چروک داره؟ 😱😱😱😱😱😱</t>
   </si>
   <si>
     <t>weird_.woman</t>
+  </si>
+  <si>
+    <t>❤️❤️❤️</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>#امیدوارم_هر_برگی_که_از_درخت_می_افتد_آمینی_باشد_بر_استجابت_آرزوهایتان</t>
@@ -164,16 +164,16 @@
     <t>0</t>
   </si>
   <si>
+    <t>ماری جون بیا از گوشواره های خوشگل من خرید کن😍</t>
+  </si>
+  <si>
+    <t>gaallery.aram</t>
+  </si>
+  <si>
     <t>مثل همیشه خوشگل وجذاب 😍😍👏👏</t>
   </si>
   <si>
     <t>masoumeh4840</t>
-  </si>
-  <si>
-    <t>ماری جون بیا از گوشواره های خوشگل من خرید کن😍</t>
-  </si>
-  <si>
-    <t>gaallery.aram</t>
   </si>
 </sst>
 </file>
@@ -603,10 +603,10 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -617,10 +617,10 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -760,7 +760,7 @@
         <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -788,7 +788,7 @@
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -802,7 +802,7 @@
         <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>